<commit_message>
lots of todo items accomplished (see readme)
</commit_message>
<xml_diff>
--- a/resources/spreadsheets/backgrounds.xlsx
+++ b/resources/spreadsheets/backgrounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="backgrounds" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4358" uniqueCount="1150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4362" uniqueCount="1150">
   <si>
     <t xml:space="preserve">bid</t>
   </si>
@@ -3761,7 +3761,7 @@
   <dimension ref="A1:V50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S62" activeCellId="1" sqref="H2:H172 S62"/>
+      <selection pane="topLeft" activeCell="S62" activeCellId="0" sqref="S62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6955,10 +6955,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N173"/>
+  <dimension ref="A1:N175"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A108" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I173" activeCellId="1" sqref="H2:H172 I173"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A129" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I173" activeCellId="0" sqref="I173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13423,6 +13423,10 @@
         <f aca="false">_xlfn.CONCAT("('",C172,"','",E172,"','",F172,"'),")</f>
         <v>('4','62',''),</v>
       </c>
+      <c r="I172" s="1" t="str">
+        <f aca="false">IF(G172="","",_xlfn.CONCAT("('",A172,"','",G172,"'),"))</f>
+        <v/>
+      </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="n">
@@ -13445,6 +13449,70 @@
       <c r="H173" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("('",C173,"','",E173,"','",F173,"'),")</f>
         <v>('16','62',''),</v>
+      </c>
+      <c r="I173" s="1" t="str">
+        <f aca="false">IF(G173="","",_xlfn.CONCAT("('",A173,"','",G173,"'),"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C174" s="1" t="n">
+        <f aca="false">INDEX(K$2:K$50,MATCH(B174,L$2:L$50,0),1)</f>
+        <v>24</v>
+      </c>
+      <c r="D174" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E174" s="1" t="n">
+        <f aca="false">INDEX(M$2:M$168,MATCH(D174,N$2:N$168,0),1)</f>
+        <v>2</v>
+      </c>
+      <c r="G174" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="H174" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("('",C174,"','",E174,"','",F174,"'),")</f>
+        <v>('24','2',''),</v>
+      </c>
+      <c r="I174" s="1" t="str">
+        <f aca="false">IF(G174="","",_xlfn.CONCAT("('",A174,"','",G174,"'),"))</f>
+        <v>('173','174'),</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C175" s="1" t="n">
+        <f aca="false">INDEX(K$2:K$50,MATCH(B175,L$2:L$50,0),1)</f>
+        <v>24</v>
+      </c>
+      <c r="D175" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E175" s="1" t="n">
+        <f aca="false">INDEX(M$2:M$168,MATCH(D175,N$2:N$168,0),1)</f>
+        <v>34</v>
+      </c>
+      <c r="G175" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="H175" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("('",C175,"','",E175,"','",F175,"'),")</f>
+        <v>('24','34',''),</v>
+      </c>
+      <c r="I175" s="1" t="str">
+        <f aca="false">IF(G175="","",_xlfn.CONCAT("('",A175,"','",G175,"'),"))</f>
+        <v>('174','173'),</v>
       </c>
     </row>
   </sheetData>
@@ -13466,7 +13534,7 @@
   <dimension ref="A1:Q171"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J98" activeCellId="1" sqref="H2:H172 J98"/>
+      <selection pane="topLeft" activeCell="J98" activeCellId="0" sqref="J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19047,8 +19115,8 @@
   </sheetPr>
   <dimension ref="A1:M707"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A143" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H172"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A143" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -28559,7 +28627,7 @@
   <dimension ref="A1:M651"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H42" activeCellId="0" sqref="H2:H172"/>
+      <selection pane="topLeft" activeCell="H42" activeCellId="0" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34278,7 +34346,7 @@
   <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="H2:H172 G2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -35359,7 +35427,7 @@
   <dimension ref="A1:L115"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H2:H172"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>